<commit_message>
Atualização automática de SAO_VALENTIM.xlsx
</commit_message>
<xml_diff>
--- a/SAO_VALENTIM.xlsx
+++ b/SAO_VALENTIM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BEB80905-65A7-44A4-9948-54B75DBB96F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D830D67-C300-4721-B226-B5584AAB391E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1201,7 +1201,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{7DC4676D-A553-4E60-AF35-6567DD8D44B7}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{9BECB262-9683-43C1-A715-038AFE20C2FF}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1231,10 +1231,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5007E7F5-2797-4497-B4D1-914F879AA85D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9464EF78-EF05-4772-91EB-569AFC8CD056}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1272,7 +1272,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{827EA056-3608-4343-8576-5536D88447B5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{670720E8-AE3D-4A16-B12C-1DCD15B90F95}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1335,7 +1335,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16D22234-3134-4C53-B887-CB60A448FAFE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18CAC2E2-ACD6-469D-8617-E981D09C57F2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1354,7 +1354,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{846784C9-30ED-51EC-0D27-58CC4AFDAF81}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CEB1EDB-780B-5C82-2095-4EFD0223360D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1403,7 +1403,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2A232D8-79E6-11C7-7E55-077FD7506877}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D32354D6-3137-F3CC-8314-C526CCAB7F13}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1422,7 +1422,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78576FD0-E00D-D2E0-243F-67CA003262AE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D243BAF-56E6-D805-DFBD-1110AB92B094}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1453,7 +1453,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B08B7BB3-CA22-F389-E4D9-DB638AD3AB73}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4514332A-4BB5-F289-DA75-287BCD82A804}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1484,7 +1484,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF6EB4EB-FABF-81F7-C8DD-FE38A1F7CC69}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AADDC96F-6CEC-C517-A760-943DAC7942F4}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1527,7 +1527,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFA70D99-D3DF-4122-9168-E2DCED8E1365}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDFBDCC4-1C98-41A7-BB55-4CEBA642E666}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1565,7 +1565,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1124277-EE2C-449A-A6FD-A7C930C67C52}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B294FAC3-BAD7-44AA-9598-120C90F2AF11}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1608,7 +1608,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4031503-3653-4F7B-93C1-5080196BB204}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36ECCFA3-14C7-4B4C-9423-AC8607A03811}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1921,7 +1921,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44E4A76A-96D9-4D63-AB1F-106E1AB050BE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66D82DB8-123F-4BBA-B014-F5A4D8475019}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>